<commit_message>
Corrected data for risks 35, 37 * 39
</commit_message>
<xml_diff>
--- a/clensed.xlsx
+++ b/clensed.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PythonProjects\clensed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4995E65A-86A3-4935-9CA5-0EE7F189B513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BCD268-773E-4DFB-BBF0-79FB143F6F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clensed" sheetId="1" r:id="rId1"/>
@@ -1747,7 +1747,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2589,12 +2589,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A40" sqref="A40"/>
+      <selection pane="topRight" activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5819,6 +5819,12 @@
       <c r="J38" t="s">
         <v>209</v>
       </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
       <c r="M38" t="s">
         <v>379</v>
       </c>
@@ -5845,6 +5851,12 @@
       </c>
       <c r="U38" t="s">
         <v>46</v>
+      </c>
+      <c r="V38">
+        <v>2</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
       </c>
       <c r="X38" t="s">
         <v>47</v>
@@ -5961,6 +5973,12 @@
       <c r="J40" t="s">
         <v>209</v>
       </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>3</v>
+      </c>
       <c r="M40" t="s">
         <v>395</v>
       </c>
@@ -5989,10 +6007,10 @@
         <v>46</v>
       </c>
       <c r="V40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X40" t="s">
         <v>47</v>
@@ -6109,6 +6127,12 @@
       <c r="J42" t="s">
         <v>209</v>
       </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>2</v>
+      </c>
       <c r="M42" t="s">
         <v>414</v>
       </c>
@@ -6135,6 +6159,12 @@
       </c>
       <c r="U42" t="s">
         <v>46</v>
+      </c>
+      <c r="V42">
+        <v>2</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
       </c>
       <c r="X42" t="s">
         <v>47</v>

</xml_diff>